<commit_message>
i have add all file and do some modification
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project learning\file demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CAE933-8A4E-4406-A252-88521379B9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B40BA3-3D76-4668-A8CA-717A0CA61609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>rishu</t>
   </si>
   <si>
     <t>hello</t>
+  </si>
+  <si>
+    <t>hi</t>
   </si>
 </sst>
 </file>
@@ -351,7 +354,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -366,6 +369,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I13" t="s">
         <v>0</v>

</xml_diff>